<commit_message>
Se registra incidencia indicadores
Ana 12102022
</commit_message>
<xml_diff>
--- a/Bitacora Incidencias_A.xlsx
+++ b/Bitacora Incidencias_A.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gdiazle\Documents\GitHub\DocEjecucionBots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7457696A-FE6D-483C-92E9-C837A06445A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971FEC58-287B-48B5-A977-6CC0BBCB8402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{72B84A4B-976C-4D7E-B731-EC25B8186A46}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="3" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$2:$I$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja2!$A$2:$I$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,6 +39,33 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>mediazb</author>
+  </authors>
+  <commentList>
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{4043EA63-DFF6-4D40-BC58-EDBC8BF23163}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">**Atendida: Se revisó pero no se quito el error
+**Resuelta: Se quito el error y no se tienen dudas
+**Pendiente de Respuesta
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>mediazb</author>
@@ -66,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="99">
   <si>
     <t>FECHA</t>
   </si>
@@ -236,135 +263,6 @@
     <t>70 Catalogo Clientes (88)</t>
   </si>
   <si>
-    <t>159 3 Seguimiento Saldos CC</t>
-  </si>
-  <si>
-    <t>159 3 Seguimiento Saldos</t>
-  </si>
-  <si>
-    <t>159 2 Seguimiento HDR CC</t>
-  </si>
-  <si>
-    <t>159 2 Seguimiento HDR</t>
-  </si>
-  <si>
-    <t>159 1 Remisiones Detalle CC</t>
-  </si>
-  <si>
-    <t>159 1 Remisiones Detalle</t>
-  </si>
-  <si>
-    <t>Indicador 88_Global Transacciones</t>
-  </si>
-  <si>
-    <t>64_5_Pendientes_por_Recolectar</t>
-  </si>
-  <si>
-    <t>Pendientes_TWI_56_4_TWI</t>
-  </si>
-  <si>
-    <t>Modificado y cancelado_44_Concentrado_TWI_MC</t>
-  </si>
-  <si>
-    <t>97 4 Faltantes Suc Producto Nuevo_CC</t>
-  </si>
-  <si>
-    <t>97 4 Faltantes Suc Producto Nuevo</t>
-  </si>
-  <si>
-    <t>97 3 Devolucion_No_Facturada_Sucursales_CC</t>
-  </si>
-  <si>
-    <t>97 3 Devolucion_No_Facturada_Sucursales</t>
-  </si>
-  <si>
-    <t>97 2 Entrega Editores_CC</t>
-  </si>
-  <si>
-    <t>97 2 Entrega Editores</t>
-  </si>
-  <si>
-    <t>97 1 Envio Sucursales</t>
-  </si>
-  <si>
-    <t>109_Cortesias_CC</t>
-  </si>
-  <si>
-    <t>109_Cortesias</t>
-  </si>
-  <si>
-    <t>99_88_8_Entradas_MC</t>
-  </si>
-  <si>
-    <t>90_0_Plantilla_Lotes_Devolucion</t>
-  </si>
-  <si>
-    <t>70 Catalogo Clientes</t>
-  </si>
-  <si>
-    <t>69 Descriptivas</t>
-  </si>
-  <si>
-    <t>41_2_Rep_Dif_Pedidos</t>
-  </si>
-  <si>
-    <t>41_Reporte_Diferencias_Pedidos_CC</t>
-  </si>
-  <si>
-    <t>41_1_Rep_Dif_Transacciones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No bajo la informacion completa </t>
-  </si>
-  <si>
-    <t>41_1_Rep_Dif_Transacciones_CC</t>
-  </si>
-  <si>
-    <t>No aumentan las cantidades</t>
-  </si>
-  <si>
-    <t>67 Bedetails_CC</t>
-  </si>
-  <si>
-    <t>Incidencia</t>
-  </si>
-  <si>
-    <t>67 Bedetails</t>
-  </si>
-  <si>
-    <t>Correcto</t>
-  </si>
-  <si>
-    <t>106 Canceladas Remision Detalle_CC</t>
-  </si>
-  <si>
-    <t>Sin ejecutar</t>
-  </si>
-  <si>
-    <t>106 Canceladas Remision Detalle</t>
-  </si>
-  <si>
-    <t>44_0_3_Remisiones_Mod_Canc_CC</t>
-  </si>
-  <si>
-    <t>3 44_0_3_Remisiones_Mod_Canc</t>
-  </si>
-  <si>
-    <t>44_0_2_Fact_Mod_Canc_CC</t>
-  </si>
-  <si>
-    <t>44_0_2_Fact_Mod_Canc</t>
-  </si>
-  <si>
-    <t>88 Diario de ventas</t>
-  </si>
-  <si>
-    <t>88 Diario de ventas_CC</t>
-  </si>
-  <si>
-    <t>103 Detalle devoluciones</t>
-  </si>
-  <si>
     <t>44_0_3_Remisiones_Mod_Canc_CC (88)</t>
   </si>
   <si>
@@ -450,13 +348,55 @@
   </si>
   <si>
     <t>Alex ejecuta el SP por medio del SQL. Comenta que el error viene del tiempo del proceso, se lo comentará a César para dar solución.</t>
+  </si>
+  <si>
+    <t>97 1 Envio Sucursales_CC (88)</t>
+  </si>
+  <si>
+    <t>Error al cargar los datos en 3000 controles</t>
+  </si>
+  <si>
+    <t>Dado que la modificación del proyecto lo lleva acabo César, se le comentará el día de mañana 20/09/2022</t>
+  </si>
+  <si>
+    <t>Pendiente de respuesta</t>
+  </si>
+  <si>
+    <t>Se hace prueba en el proyecto y vuelve a arrojar una cantidad mayor a la tendencia, en este caso fue duplicar los datos</t>
+  </si>
+  <si>
+    <t>César pide verificar el GitHub para saber sí se ha descargado la última versión en la computadora de Ana. Dado que es correcto pide ejecutar nuevamente el autoit, no se tiene ningún error.</t>
+  </si>
+  <si>
+    <t>Atendida, aún se tienen dudas.</t>
+  </si>
+  <si>
+    <t>Al validar la información en 3000 controles se encuentra una diferencia de 5 millones por arriba con la cifra de la semana pasada, algo que no es tendencial con el alza de las cifras en semanas anteriores.</t>
+  </si>
+  <si>
+    <t>Indicadores de Proyecto 88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error al actualizar los datos </t>
+  </si>
+  <si>
+    <t>Ana // Paloma</t>
+  </si>
+  <si>
+    <t>César // Rafael</t>
+  </si>
+  <si>
+    <t>Cuando se manda a actualizar el indicador envía el error de SQL y no permite actualizarlo.</t>
+  </si>
+  <si>
+    <t>Pendiente de Respuesta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -485,14 +425,8 @@
       <name val="Britannic Bold"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -505,44 +439,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -630,26 +528,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -685,17 +568,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -712,30 +584,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1050,13 +899,593 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4DD5CBE-D75F-430E-80BF-54955A4C5430}">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFE8874-8752-49EC-9620-21644F94EDCF}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="45" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>44846</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="11"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="11"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="11"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="11"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="11"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="11"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="11"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="11"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="11"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="11"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="11"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="11"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="6"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="6"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="6"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="6"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="6"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="6"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="6"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="6"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="6"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="6"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="6"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="6"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="6"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="6"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="6"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="6"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4DD5CBE-D75F-430E-80BF-54955A4C5430}">
+  <dimension ref="A1:I47"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,17 +1500,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="27"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
@@ -1112,7 +1541,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>44804</v>
       </c>
@@ -1129,7 +1558,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>11</v>
@@ -1141,7 +1570,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>44805</v>
       </c>
@@ -1158,7 +1587,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>17</v>
@@ -1170,7 +1599,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>44806</v>
       </c>
@@ -1187,7 +1616,7 @@
         <v>19</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>21</v>
@@ -1199,7 +1628,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>44809</v>
       </c>
@@ -1216,7 +1645,7 @@
         <v>19</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>30</v>
@@ -1228,7 +1657,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>44809</v>
       </c>
@@ -1245,7 +1674,7 @@
         <v>10</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>28</v>
@@ -1257,7 +1686,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>44809</v>
       </c>
@@ -1274,7 +1703,7 @@
         <v>10</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>31</v>
@@ -1286,7 +1715,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>44809</v>
       </c>
@@ -1303,7 +1732,7 @@
         <v>19</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>34</v>
@@ -1315,7 +1744,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>44810</v>
       </c>
@@ -1344,7 +1773,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>44810</v>
       </c>
@@ -1361,7 +1790,7 @@
         <v>19</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>53</v>
@@ -1373,7 +1802,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>44810</v>
       </c>
@@ -1402,7 +1831,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>44810</v>
       </c>
@@ -1431,7 +1860,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>44811</v>
       </c>
@@ -1439,10 +1868,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>10</v>
@@ -1451,16 +1880,16 @@
         <v>43</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>101</v>
+        <v>58</v>
       </c>
       <c r="I14" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>44811</v>
       </c>
@@ -1471,25 +1900,25 @@
         <v>8</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>105</v>
+        <v>62</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="I15" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>44811</v>
       </c>
@@ -1500,25 +1929,25 @@
         <v>8</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>107</v>
+        <v>64</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>108</v>
+        <v>65</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>109</v>
+        <v>66</v>
       </c>
       <c r="I16" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>44816</v>
       </c>
@@ -1526,7 +1955,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="4" t="s">
@@ -1539,7 +1968,7 @@
       <c r="H17" s="5"/>
       <c r="I17" s="11"/>
     </row>
-    <row r="18" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>44816</v>
       </c>
@@ -1547,10 +1976,10 @@
         <v>2</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>19</v>
@@ -1559,16 +1988,16 @@
         <v>43</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>113</v>
+        <v>70</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>114</v>
+        <v>71</v>
       </c>
       <c r="I18" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>44817</v>
       </c>
@@ -1579,54 +2008,54 @@
         <v>55</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>117</v>
+        <v>74</v>
       </c>
       <c r="I19" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>44817</v>
       </c>
       <c r="B20" s="4">
         <v>2</v>
       </c>
-      <c r="C20" s="24" t="s">
-        <v>118</v>
+      <c r="C20" s="13" t="s">
+        <v>75</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>119</v>
+        <v>76</v>
       </c>
       <c r="I20" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>44817</v>
       </c>
@@ -1634,25 +2063,25 @@
         <v>3</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>120</v>
+        <v>77</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>121</v>
+        <v>78</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>123</v>
+        <v>80</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>124</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1666,7 +2095,7 @@
         <v>55</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>125</v>
+        <v>82</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>19</v>
@@ -1675,36 +2104,72 @@
         <v>43</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>127</v>
+        <v>84</v>
       </c>
       <c r="I22" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="6"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="6"/>
+    <row r="23" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
+        <v>44823</v>
+      </c>
+      <c r="B23" s="4">
+        <v>2</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
+        <v>44824</v>
+      </c>
+      <c r="B24" s="4">
+        <v>1</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
@@ -1960,13 +2425,7 @@
       <c r="I47" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:I22" xr:uid="{E4DD5CBE-D75F-430E-80BF-54955A4C5430}">
-    <filterColumn colId="0">
-      <filters>
-        <dateGroupItem year="2022" month="9" day="19" dateTimeGrouping="day"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:I24" xr:uid="{E4DD5CBE-D75F-430E-80BF-54955A4C5430}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
@@ -1974,238 +2433,4 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D39D5E9D-01AD-43B3-B2B4-EF8519DE3BF3}">
-  <dimension ref="A1:D38"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="48" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="C8" s="23"/>
-      <c r="D8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" s="22"/>
-      <c r="D9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" s="21"/>
-      <c r="D10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="19"/>
-      <c r="D12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A1:A38">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>ROW()=CELL("fila")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>